<commit_message>
fix bugs for delete row and load form with no predefined commands
</commit_message>
<xml_diff>
--- a/src/main/resources/websheet/PRICELISTINPUT.xlsx
+++ b/src/main/resources/websheet/PRICELISTINPUT.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="13080" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="Sale Price Report" sheetId="1" r:id="rId1"/>
-    <sheet name="Configuration" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Sale Price Report'!$A$1:$F$9</definedName>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Sale Price Report</t>
   </si>
@@ -73,85 +72,13 @@
       <t>Jason.Jiang.ca@gmail.com</t>
     </r>
   </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>Tab Name</t>
-  </si>
-  <si>
-    <t>Sheet Name</t>
-  </si>
-  <si>
-    <t>Form Header Range</t>
-  </si>
-  <si>
-    <t>Form Body Range</t>
-  </si>
-  <si>
-    <t>Form Footer Range</t>
-  </si>
-  <si>
-    <t>Form Body Type</t>
-  </si>
-  <si>
-    <t>Allow ADD/DELETE ROW</t>
-  </si>
-  <si>
-    <t>Initial Rows</t>
-  </si>
-  <si>
-    <t>Form Page Type</t>
-  </si>
-  <si>
-    <t>Form Width</t>
-  </si>
-  <si>
-    <t>Max Rows Per Page</t>
-  </si>
-  <si>
-    <t>Saved Rows Before Repeat</t>
-  </si>
-  <si>
-    <t>Saved Rows After Repeat</t>
-  </si>
-  <si>
-    <t>Target Column/Cell</t>
-  </si>
-  <si>
-    <t>Attributes Type</t>
-  </si>
-  <si>
-    <t>Attributes Value</t>
-  </si>
-  <si>
-    <t>Validation Error Messages</t>
-  </si>
-  <si>
-    <t>$A$3 : $F$5</t>
-  </si>
-  <si>
-    <t>$A$6 : $F$9</t>
-  </si>
-  <si>
-    <t>Repeat</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="25" x14ac:knownFonts="1">
     <font>
@@ -694,27 +621,9 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="24" borderId="0" xfId="41" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="24" borderId="0" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -744,7 +653,7 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="5" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -759,7 +668,7 @@
     <xf numFmtId="1" fontId="5" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="5" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1142,120 +1051,120 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="23" style="2" customWidth="1"/>
-    <col min="5" max="5" width="27.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="23.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="6.1640625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.33203125" style="2"/>
+    <col min="1" max="1" width="10.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" ht="0.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="F2" s="9"/>
+    <row r="2" spans="1:6" ht="0.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+    <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
     </row>
-    <row r="4" spans="1:6" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="26"/>
-      <c r="F4" s="27"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="21"/>
     </row>
-    <row r="5" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="11" t="s">
+    <row r="5" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="8" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12">
+    <row r="6" spans="1:6" s="2" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
         <f>ROW()-5</f>
         <v>1</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16">
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10">
         <f>$D$6*$E$6</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="8" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
+    <row r="7" spans="1:6" s="2" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20">
+      <c r="B7" s="6"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14">
         <f ca="1">SUM(INDIRECT("E6"):INDIRECT("E"&amp;TEXT(ROW()-1,"0")))</f>
         <v>0</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="15">
         <f ca="1">SUM(INDIRECT("F6"):INDIRECT("F"&amp;TEXT(ROW()-1,"0")))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
+    <row r="8" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
     </row>
-    <row r="9" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
+    <row r="9" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -1273,131 +1182,4 @@
   <pageSetup scale="55" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="11.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="2" customWidth="1"/>
-    <col min="5" max="6" width="16.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="22.1640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="29" style="3" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="33.83203125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="43.6640625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="57.1640625" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-    </row>
-  </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <pageMargins left="0.69861111111111107" right="0.69861111111111107" top="0.75" bottom="0.75" header="0.51111111111111107" footer="0.51111111111111107"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
 </file>
</xml_diff>